<commit_message>
Ajustes varios al archivo del modelo de energía por parte de UCR/USFQ (1).
</commit_message>
<xml_diff>
--- a/Energia/Model/t1_confection/A1_Outputs/A-O_AR_Model_Base_Year.xlsx
+++ b/Energia/Model/t1_confection/A1_Outputs/A-O_AR_Model_Base_Year.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luisf\Dropbox\2_WORK\EperLab\2_Herramientas\_mmf_ECU\modelo_energia_202210\t1_confection_v23\A1_Outputs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ucr\Desktop\t1_confection_v23\A1_Outputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{983D5B95-995C-42D2-897C-8DE0FE29218D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99D2B319-93B9-4140-9E3F-E229DD4555D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Primary" sheetId="1" r:id="rId1"/>
@@ -209,7 +209,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1884" uniqueCount="794">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1892" uniqueCount="798">
   <si>
     <t>Tech</t>
   </si>
@@ -2591,6 +2591,18 @@
   </si>
   <si>
     <t>TRNCRU</t>
+  </si>
+  <si>
+    <t>E1_ELE_FF</t>
+  </si>
+  <si>
+    <t>PP_TPP</t>
+  </si>
+  <si>
+    <t>Thermal power plants</t>
+  </si>
+  <si>
+    <t>Thermal Electricity</t>
   </si>
 </sst>
 </file>
@@ -3552,17 +3564,17 @@
       <selection pane="bottomLeft" activeCell="A10" sqref="A3:F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.23046875" customWidth="1"/>
-    <col min="2" max="2" width="70.3046875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.3046875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.84375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.69140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.53515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.28515625" customWidth="1"/>
+    <col min="2" max="2" width="70.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3582,7 +3594,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" hidden="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>732</v>
       </c>
@@ -3602,7 +3614,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>6</v>
       </c>
@@ -3622,7 +3634,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:6" hidden="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>11</v>
       </c>
@@ -3642,7 +3654,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:6" hidden="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>15</v>
       </c>
@@ -3662,7 +3674,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:6" hidden="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>19</v>
       </c>
@@ -3682,7 +3694,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:6" hidden="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>23</v>
       </c>
@@ -3702,7 +3714,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:6" hidden="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>27</v>
       </c>
@@ -3722,7 +3734,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:6" hidden="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>31</v>
       </c>
@@ -3742,7 +3754,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>35</v>
       </c>
@@ -3762,7 +3774,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:6" hidden="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
         <v>38</v>
       </c>
@@ -3782,7 +3794,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:6" hidden="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>42</v>
       </c>
@@ -3802,7 +3814,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:6" hidden="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
         <v>46</v>
       </c>
@@ -3822,7 +3834,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:6" hidden="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
         <v>54</v>
       </c>
@@ -3842,7 +3854,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:6" hidden="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
         <v>56</v>
       </c>
@@ -3862,7 +3874,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:6" hidden="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
         <v>60</v>
       </c>
@@ -3882,7 +3894,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:6" hidden="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
         <v>64</v>
       </c>
@@ -3902,7 +3914,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:6" hidden="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
         <v>68</v>
       </c>
@@ -3922,7 +3934,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:6" hidden="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
         <v>72</v>
       </c>
@@ -3942,7 +3954,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:6" hidden="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
         <v>76</v>
       </c>
@@ -3962,7 +3974,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:6" hidden="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
         <v>78</v>
       </c>
@@ -3982,7 +3994,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:6" hidden="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
         <v>80</v>
       </c>
@@ -4002,7 +4014,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:6" hidden="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
         <v>82</v>
       </c>
@@ -4022,7 +4034,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:6" hidden="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
         <v>84</v>
       </c>
@@ -4042,7 +4054,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="1:6" hidden="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
         <v>86</v>
       </c>
@@ -4062,7 +4074,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:6" hidden="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
         <v>88</v>
       </c>
@@ -4082,7 +4094,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:6" hidden="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="9" t="s">
         <v>90</v>
       </c>
@@ -4102,7 +4114,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:6" hidden="1" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="9" t="s">
         <v>92</v>
       </c>
@@ -4122,7 +4134,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="1:6" hidden="1" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="9" t="s">
         <v>94</v>
       </c>
@@ -4142,7 +4154,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="30" spans="1:6" hidden="1" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="9" t="s">
         <v>96</v>
       </c>
@@ -4162,7 +4174,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="31" spans="1:6" hidden="1" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="9" t="s">
         <v>98</v>
       </c>
@@ -4182,7 +4194,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="32" spans="1:6" hidden="1" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="9" t="s">
         <v>100</v>
       </c>
@@ -4202,7 +4214,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="33" spans="1:6" hidden="1" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="9" t="s">
         <v>102</v>
       </c>
@@ -4222,7 +4234,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="34" spans="1:6" hidden="1" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="9" t="s">
         <v>104</v>
       </c>
@@ -4242,7 +4254,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="35" spans="1:6" hidden="1" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="9" t="s">
         <v>106</v>
       </c>
@@ -4262,7 +4274,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="36" spans="1:6" hidden="1" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" s="9" t="s">
         <v>108</v>
       </c>
@@ -4282,7 +4294,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="37" spans="1:6" hidden="1" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" s="9" t="s">
         <v>111</v>
       </c>
@@ -4302,7 +4314,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="38" spans="1:6" hidden="1" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" s="9" t="s">
         <v>114</v>
       </c>
@@ -4322,7 +4334,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="39" spans="1:6" hidden="1" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" s="9" t="s">
         <v>116</v>
       </c>
@@ -4342,7 +4354,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="40" spans="1:6" hidden="1" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" s="9" t="s">
         <v>118</v>
       </c>
@@ -4362,7 +4374,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="41" spans="1:6" hidden="1" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" s="9" t="s">
         <v>120</v>
       </c>
@@ -4382,7 +4394,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="42" spans="1:6" hidden="1" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" s="9" t="s">
         <v>122</v>
       </c>
@@ -4402,7 +4414,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="43" spans="1:6" hidden="1" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" s="9" t="s">
         <v>124</v>
       </c>
@@ -4422,7 +4434,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="44" spans="1:6" hidden="1" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" s="9" t="s">
         <v>126</v>
       </c>
@@ -4442,7 +4454,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="45" spans="1:6" hidden="1" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" s="9" t="s">
         <v>128</v>
       </c>
@@ -4462,7 +4474,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="46" spans="1:6" hidden="1" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" s="9" t="s">
         <v>130</v>
       </c>
@@ -4498,28 +4510,28 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:J59"/>
+  <dimension ref="A1:J60"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G57" sqref="G57"/>
+      <selection pane="bottomLeft" activeCell="F54" sqref="F54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.3046875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35.84375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.69140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.4609375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="75.4609375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.23046875" customWidth="1"/>
-    <col min="8" max="8" width="35.84375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.69140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.53515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="75.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.28515625" customWidth="1"/>
+    <col min="8" max="8" width="35.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>132</v>
       </c>
@@ -4551,7 +4563,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:10" hidden="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
         <v>113</v>
       </c>
@@ -4583,7 +4595,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
         <v>173</v>
       </c>
@@ -4603,10 +4615,10 @@
         <v>198</v>
       </c>
       <c r="G3" s="19" t="s">
-        <v>74</v>
+        <v>794</v>
       </c>
       <c r="H3" s="19" t="s">
-        <v>75</v>
+        <v>797</v>
       </c>
       <c r="I3" s="19">
         <v>1</v>
@@ -4615,7 +4627,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
         <v>173</v>
       </c>
@@ -4647,7 +4659,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
         <v>173</v>
       </c>
@@ -4679,7 +4691,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
         <v>173</v>
       </c>
@@ -4711,7 +4723,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:10" hidden="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
         <v>173</v>
       </c>
@@ -4743,7 +4755,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:10" hidden="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="21" t="s">
         <v>244</v>
       </c>
@@ -4775,7 +4787,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:10" hidden="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="21" t="s">
         <v>142</v>
       </c>
@@ -4807,7 +4819,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:10" hidden="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="21" t="s">
         <v>142</v>
       </c>
@@ -4839,7 +4851,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:10" hidden="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="21" t="s">
         <v>17</v>
       </c>
@@ -4871,7 +4883,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="21" t="s">
         <v>13</v>
       </c>
@@ -4891,10 +4903,10 @@
         <v>194</v>
       </c>
       <c r="G12" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="H12" s="11" t="s">
-        <v>75</v>
+        <v>794</v>
+      </c>
+      <c r="H12" s="19" t="s">
+        <v>797</v>
       </c>
       <c r="I12" s="11">
         <v>1</v>
@@ -4903,7 +4915,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="21" t="s">
         <v>13</v>
       </c>
@@ -4923,10 +4935,10 @@
         <v>196</v>
       </c>
       <c r="G13" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="H13" s="11" t="s">
-        <v>75</v>
+        <v>794</v>
+      </c>
+      <c r="H13" s="19" t="s">
+        <v>797</v>
       </c>
       <c r="I13" s="11">
         <v>1</v>
@@ -4935,7 +4947,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="21" t="s">
         <v>13</v>
       </c>
@@ -4967,7 +4979,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="21" t="s">
         <v>13</v>
       </c>
@@ -4999,7 +5011,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="21" t="s">
         <v>13</v>
       </c>
@@ -5031,7 +5043,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="21" t="s">
         <v>13</v>
       </c>
@@ -5063,7 +5075,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="21" t="s">
         <v>13</v>
       </c>
@@ -5095,7 +5107,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="21" t="s">
         <v>13</v>
       </c>
@@ -5127,7 +5139,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:10" hidden="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="21" t="s">
         <v>13</v>
       </c>
@@ -5159,7 +5171,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:10" hidden="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="21" t="s">
         <v>173</v>
       </c>
@@ -5191,7 +5203,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:10" hidden="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="21" t="s">
         <v>173</v>
       </c>
@@ -5223,7 +5235,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="21" t="s">
         <v>29</v>
       </c>
@@ -5255,7 +5267,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="21" t="s">
         <v>29</v>
       </c>
@@ -5275,10 +5287,10 @@
         <v>190</v>
       </c>
       <c r="G24" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="H24" s="11" t="s">
-        <v>75</v>
+        <v>794</v>
+      </c>
+      <c r="H24" s="19" t="s">
+        <v>797</v>
       </c>
       <c r="I24" s="11">
         <v>1</v>
@@ -5287,7 +5299,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="21" t="s">
         <v>29</v>
       </c>
@@ -5307,10 +5319,10 @@
         <v>192</v>
       </c>
       <c r="G25" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="H25" s="11" t="s">
-        <v>75</v>
+        <v>794</v>
+      </c>
+      <c r="H25" s="19" t="s">
+        <v>797</v>
       </c>
       <c r="I25" s="11">
         <v>1</v>
@@ -5319,7 +5331,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:10" hidden="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="21" t="s">
         <v>235</v>
       </c>
@@ -5351,7 +5363,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:10" hidden="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="21" t="s">
         <v>74</v>
       </c>
@@ -5383,7 +5395,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:10" hidden="1" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="11" t="s">
         <v>767</v>
       </c>
@@ -5415,7 +5427,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="1:10" hidden="1" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="21" t="s">
         <v>13</v>
       </c>
@@ -5447,7 +5459,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="30" spans="1:10" hidden="1" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="21" t="s">
         <v>29</v>
       </c>
@@ -5479,7 +5491,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="31" spans="1:10" hidden="1" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="21" t="s">
         <v>33</v>
       </c>
@@ -5511,7 +5523,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="32" spans="1:10" hidden="1" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="21" t="s">
         <v>170</v>
       </c>
@@ -5543,7 +5555,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="33" spans="1:10" hidden="1" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="11" t="s">
         <v>37</v>
       </c>
@@ -5575,7 +5587,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="34" spans="1:10" hidden="1" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="11" t="s">
         <v>792</v>
       </c>
@@ -5607,7 +5619,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="35" spans="1:10" hidden="1" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="11" t="s">
         <v>792</v>
       </c>
@@ -5639,7 +5651,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="36" spans="1:10" hidden="1" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" s="11" t="s">
         <v>792</v>
       </c>
@@ -5671,7 +5683,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="37" spans="1:10" hidden="1" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" s="11" t="s">
         <v>792</v>
       </c>
@@ -5703,7 +5715,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="38" spans="1:10" hidden="1" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" s="11" t="s">
         <v>792</v>
       </c>
@@ -5735,7 +5747,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="39" spans="1:10" hidden="1" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" s="11" t="s">
         <v>792</v>
       </c>
@@ -5767,7 +5779,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="40" spans="1:10" hidden="1" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" s="11" t="s">
         <v>792</v>
       </c>
@@ -5799,7 +5811,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="41" spans="1:10" hidden="1" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" s="11" t="s">
         <v>792</v>
       </c>
@@ -5831,7 +5843,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="11" t="s">
         <v>767</v>
       </c>
@@ -5851,10 +5863,10 @@
         <v>200</v>
       </c>
       <c r="G42" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="H42" s="11" t="s">
-        <v>75</v>
+        <v>794</v>
+      </c>
+      <c r="H42" s="19" t="s">
+        <v>797</v>
       </c>
       <c r="I42" s="11">
         <v>1</v>
@@ -5863,7 +5875,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" s="11" t="s">
         <v>767</v>
       </c>
@@ -5895,7 +5907,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" s="11" t="s">
         <v>767</v>
       </c>
@@ -5927,7 +5939,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="45" spans="1:10" hidden="1" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" s="21" t="s">
         <v>227</v>
       </c>
@@ -5959,7 +5971,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="21" t="s">
         <v>44</v>
       </c>
@@ -5991,7 +6003,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="21" t="s">
         <v>58</v>
       </c>
@@ -6023,7 +6035,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="21" t="s">
         <v>58</v>
       </c>
@@ -6055,7 +6067,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="21" t="s">
         <v>58</v>
       </c>
@@ -6087,7 +6099,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="50" spans="1:10" hidden="1" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" s="21" t="s">
         <v>58</v>
       </c>
@@ -6119,7 +6131,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="51" spans="1:10" hidden="1" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" s="21" t="s">
         <v>52</v>
       </c>
@@ -6151,7 +6163,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="52" spans="1:10" hidden="1" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" s="21" t="s">
         <v>8</v>
       </c>
@@ -6183,7 +6195,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" s="21" t="s">
         <v>21</v>
       </c>
@@ -6203,10 +6215,10 @@
         <v>188</v>
       </c>
       <c r="G53" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="H53" s="11" t="s">
-        <v>75</v>
+        <v>794</v>
+      </c>
+      <c r="H53" s="19" t="s">
+        <v>797</v>
       </c>
       <c r="I53" s="11">
         <v>1</v>
@@ -6215,7 +6227,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" s="21" t="s">
         <v>66</v>
       </c>
@@ -6247,7 +6259,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="55" spans="1:10" hidden="1" x14ac:dyDescent="0.4">
+    <row r="55" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" s="21" t="s">
         <v>66</v>
       </c>
@@ -6279,7 +6291,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="56" spans="1:10" hidden="1" x14ac:dyDescent="0.4">
+    <row r="56" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" s="21" t="s">
         <v>66</v>
       </c>
@@ -6311,7 +6323,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" s="21" t="s">
         <v>70</v>
       </c>
@@ -6343,7 +6355,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="58" spans="1:10" hidden="1" x14ac:dyDescent="0.4">
+    <row r="58" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" s="21" t="s">
         <v>173</v>
       </c>
@@ -6375,7 +6387,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="59" spans="1:10" hidden="1" x14ac:dyDescent="0.4">
+    <row r="59" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" s="21" t="s">
         <v>173</v>
       </c>
@@ -6404,6 +6416,38 @@
         <v>1</v>
       </c>
       <c r="J59" s="12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A60" s="11" t="s">
+        <v>794</v>
+      </c>
+      <c r="B60" s="17" t="s">
+        <v>797</v>
+      </c>
+      <c r="C60" s="17">
+        <v>1</v>
+      </c>
+      <c r="D60" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="E60" s="10" t="s">
+        <v>795</v>
+      </c>
+      <c r="F60" s="10" t="s">
+        <v>796</v>
+      </c>
+      <c r="G60" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="H60" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="I60" s="11">
+        <v>1</v>
+      </c>
+      <c r="J60" s="12" t="s">
         <v>10</v>
       </c>
     </row>
@@ -6423,18 +6467,6 @@
         <filter val="PP_NGSTGS"/>
         <filter val="PP_SUG"/>
         <filter val="PP_WASICE"/>
-        <filter val="PPICRUPETICE"/>
-        <filter val="PPICRUPETTST"/>
-        <filter val="PPIDSLCEMTST"/>
-        <filter val="PPIDSLELRICE"/>
-        <filter val="PPIDSLELRTST"/>
-        <filter val="PPIDSLGALICE"/>
-        <filter val="PPIDSLPETICE"/>
-        <filter val="PPIDSLPETTGS"/>
-        <filter val="PPIFOIPETICE"/>
-        <filter val="PPINGSPETICE"/>
-        <filter val="PPINGSPETTGS"/>
-        <filter val="PPINGSPETTST"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -6452,20 +6484,20 @@
       <selection pane="bottomLeft" activeCell="E47" sqref="A32:E47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.3046875" customWidth="1"/>
-    <col min="2" max="3" width="14.4609375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.53515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.4609375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="46.69140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.84375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="44.07421875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.84375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.69140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.28515625" customWidth="1"/>
+    <col min="2" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="46.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="44.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="13" t="s">
         <v>132</v>
       </c>
@@ -6497,7 +6529,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:10" hidden="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
         <v>110</v>
       </c>
@@ -6527,7 +6559,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:10" hidden="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="21" t="s">
         <v>17</v>
       </c>
@@ -6557,7 +6589,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:10" hidden="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="21" t="s">
         <v>25</v>
       </c>
@@ -6587,7 +6619,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:10" hidden="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="21" t="s">
         <v>163</v>
       </c>
@@ -6617,7 +6649,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:10" hidden="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
         <v>110</v>
       </c>
@@ -6647,7 +6679,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:10" hidden="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="21" t="s">
         <v>13</v>
       </c>
@@ -6677,7 +6709,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:10" hidden="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="21" t="s">
         <v>17</v>
       </c>
@@ -6707,7 +6739,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:10" hidden="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="21" t="s">
         <v>33</v>
       </c>
@@ -6737,7 +6769,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:10" hidden="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="21" t="s">
         <v>25</v>
       </c>
@@ -6767,7 +6799,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:10" hidden="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="21" t="s">
         <v>163</v>
       </c>
@@ -6797,7 +6829,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:10" hidden="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="21" t="s">
         <v>13</v>
       </c>
@@ -6827,7 +6859,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:10" hidden="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="21" t="s">
         <v>110</v>
       </c>
@@ -6857,7 +6889,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:10" hidden="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="21" t="s">
         <v>29</v>
       </c>
@@ -6887,7 +6919,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:10" hidden="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="21" t="s">
         <v>17</v>
       </c>
@@ -6917,7 +6949,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:10" hidden="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="21" t="s">
         <v>25</v>
       </c>
@@ -6947,7 +6979,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:10" hidden="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="21" t="s">
         <v>13</v>
       </c>
@@ -6977,7 +7009,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:10" hidden="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="21" t="s">
         <v>110</v>
       </c>
@@ -7007,7 +7039,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:10" hidden="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="21" t="s">
         <v>48</v>
       </c>
@@ -7037,7 +7069,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:10" hidden="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="21" t="s">
         <v>29</v>
       </c>
@@ -7067,7 +7099,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:10" hidden="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="21" t="s">
         <v>17</v>
       </c>
@@ -7097,7 +7129,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:10" hidden="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="21" t="s">
         <v>256</v>
       </c>
@@ -7127,7 +7159,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:10" hidden="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="21" t="s">
         <v>40</v>
       </c>
@@ -7157,7 +7189,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:10" hidden="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="21" t="s">
         <v>25</v>
       </c>
@@ -7187,7 +7219,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="1:10" hidden="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="21" t="s">
         <v>735</v>
       </c>
@@ -7217,7 +7249,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:10" hidden="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="21" t="s">
         <v>58</v>
       </c>
@@ -7247,7 +7279,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:10" hidden="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="21" t="s">
         <v>180</v>
       </c>
@@ -7277,7 +7309,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:10" hidden="1" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="21" t="s">
         <v>110</v>
       </c>
@@ -7307,7 +7339,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="1:10" hidden="1" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="21" t="s">
         <v>48</v>
       </c>
@@ -7337,7 +7369,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="30" spans="1:10" hidden="1" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="21" t="s">
         <v>25</v>
       </c>
@@ -7367,7 +7399,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="31" spans="1:10" hidden="1" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="21" t="s">
         <v>735</v>
       </c>
@@ -7397,7 +7429,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="21" t="s">
         <v>37</v>
       </c>
@@ -7427,7 +7459,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="21" t="s">
         <v>167</v>
       </c>
@@ -7457,7 +7489,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="34" spans="1:10" hidden="1" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="21" t="s">
         <v>13</v>
       </c>
@@ -7487,7 +7519,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="35" spans="1:10" hidden="1" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="21" t="s">
         <v>74</v>
       </c>
@@ -7517,7 +7549,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="36" spans="1:10" hidden="1" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" s="21" t="s">
         <v>29</v>
       </c>
@@ -7547,7 +7579,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="37" spans="1:10" hidden="1" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" s="21" t="s">
         <v>17</v>
       </c>
@@ -7577,7 +7609,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="38" spans="1:10" hidden="1" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" s="21" t="s">
         <v>25</v>
       </c>
@@ -7607,7 +7639,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="39" spans="1:10" hidden="1" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" s="21" t="s">
         <v>66</v>
       </c>
@@ -7637,7 +7669,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="40" spans="1:10" hidden="1" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" s="21" t="s">
         <v>17</v>
       </c>
@@ -7667,7 +7699,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="41" spans="1:10" hidden="1" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" s="21" t="s">
         <v>33</v>
       </c>
@@ -7697,7 +7729,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="42" spans="1:10" hidden="1" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" s="21" t="s">
         <v>13</v>
       </c>
@@ -7727,7 +7759,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="43" spans="1:10" hidden="1" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" s="21" t="s">
         <v>29</v>
       </c>
@@ -7757,7 +7789,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="44" spans="1:10" hidden="1" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" s="22" t="s">
         <v>17</v>
       </c>
@@ -7787,7 +7819,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="45" spans="1:10" hidden="1" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" s="22" t="s">
         <v>170</v>
       </c>
@@ -7817,7 +7849,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="46" spans="1:10" hidden="1" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" s="68" t="s">
         <v>74</v>
       </c>
@@ -7847,7 +7879,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="11" t="s">
         <v>37</v>
       </c>
@@ -7877,7 +7909,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="48" spans="1:10" hidden="1" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" s="68" t="s">
         <v>17</v>
       </c>
@@ -7907,7 +7939,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="49" spans="1:10" hidden="1" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" s="11" t="s">
         <v>25</v>
       </c>
@@ -7937,7 +7969,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="50" spans="1:10" hidden="1" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" s="21" t="s">
         <v>17</v>
       </c>
@@ -7967,7 +7999,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="51" spans="1:10" hidden="1" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" s="21" t="s">
         <v>33</v>
       </c>
@@ -7997,7 +8029,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="52" spans="1:10" hidden="1" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" s="21" t="s">
         <v>13</v>
       </c>
@@ -8027,7 +8059,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="53" spans="1:10" hidden="1" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" s="21" t="s">
         <v>29</v>
       </c>
@@ -8057,7 +8089,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="54" spans="1:10" hidden="1" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" s="21" t="s">
         <v>25</v>
       </c>
@@ -8087,7 +8119,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="55" spans="1:10" hidden="1" x14ac:dyDescent="0.4">
+    <row r="55" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" s="11" t="s">
         <v>13</v>
       </c>
@@ -8117,7 +8149,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="56" spans="1:10" hidden="1" x14ac:dyDescent="0.4">
+    <row r="56" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" s="11" t="s">
         <v>33</v>
       </c>
@@ -8147,7 +8179,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="57" spans="1:10" hidden="1" x14ac:dyDescent="0.4">
+    <row r="57" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" s="11" t="s">
         <v>29</v>
       </c>
@@ -8199,21 +8231,21 @@
       <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.3046875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.07421875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.69140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.69140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="36.69140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.3046875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="37.69140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.69140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.53515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="36.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="37.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="13" t="s">
         <v>132</v>
       </c>
@@ -8245,7 +8277,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:10" hidden="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
         <v>231</v>
       </c>
@@ -8275,7 +8307,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="21" t="s">
         <v>735</v>
       </c>
@@ -8305,7 +8337,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:10" hidden="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="21" t="s">
         <v>256</v>
       </c>
@@ -8335,7 +8367,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:10" hidden="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="21" t="s">
         <v>110</v>
       </c>
@@ -8365,7 +8397,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:10" hidden="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="21" t="s">
         <v>25</v>
       </c>
@@ -8395,7 +8427,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:10" hidden="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="21" t="s">
         <v>239</v>
       </c>
@@ -8425,7 +8457,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:10" hidden="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="21" t="s">
         <v>110</v>
       </c>
@@ -8455,7 +8487,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:10" hidden="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="21" t="s">
         <v>239</v>
       </c>
@@ -8485,7 +8517,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:10" hidden="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="21" t="s">
         <v>231</v>
       </c>
@@ -8515,7 +8547,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="21" t="s">
         <v>735</v>
       </c>
@@ -8545,7 +8577,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:10" hidden="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="21" t="s">
         <v>25</v>
       </c>
@@ -8575,7 +8607,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:10" hidden="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="21" t="s">
         <v>231</v>
       </c>
@@ -8605,7 +8637,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:10" hidden="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="21" t="s">
         <v>256</v>
       </c>
@@ -8635,7 +8667,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:10" hidden="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="21" t="s">
         <v>110</v>
       </c>
@@ -8665,7 +8697,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:10" hidden="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="21" t="s">
         <v>239</v>
       </c>
@@ -8695,7 +8727,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:10" hidden="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="21" t="s">
         <v>25</v>
       </c>
@@ -8725,7 +8757,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:10" hidden="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="21" t="s">
         <v>231</v>
       </c>
@@ -8755,7 +8787,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="21" t="s">
         <v>735</v>
       </c>
@@ -8785,7 +8817,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:10" hidden="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="21" t="s">
         <v>256</v>
       </c>
@@ -8815,7 +8847,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:10" hidden="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="21" t="s">
         <v>110</v>
       </c>
@@ -8845,7 +8877,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:10" hidden="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="21" t="s">
         <v>239</v>
       </c>
@@ -8875,7 +8907,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:10" hidden="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="21" t="s">
         <v>25</v>
       </c>
@@ -8905,7 +8937,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:10" hidden="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="21" t="s">
         <v>231</v>
       </c>
@@ -8935,7 +8967,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="21" t="s">
         <v>735</v>
       </c>
@@ -8965,7 +8997,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:10" hidden="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="21" t="s">
         <v>110</v>
       </c>
@@ -8995,7 +9027,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:10" hidden="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="21" t="s">
         <v>239</v>
       </c>
@@ -9025,7 +9057,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:10" hidden="1" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="21" t="s">
         <v>25</v>
       </c>
@@ -9071,31 +9103,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:N67"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.23046875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.4609375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.23046875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.07421875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.3046875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.4609375" customWidth="1"/>
-    <col min="7" max="7" width="12.23046875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.07421875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="25.765625" customWidth="1"/>
-    <col min="10" max="10" width="32.07421875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.23046875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.69140625" customWidth="1"/>
-    <col min="13" max="13" width="11.53515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.3046875" customWidth="1"/>
-    <col min="16" max="16" width="27.84375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" customWidth="1"/>
+    <col min="7" max="7" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25.7109375" customWidth="1"/>
+    <col min="10" max="10" width="32.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.7109375" customWidth="1"/>
+    <col min="13" max="13" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.28515625" customWidth="1"/>
+    <col min="16" max="16" width="27.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="13" t="s">
         <v>537</v>
       </c>
@@ -9139,7 +9171,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="58" t="s">
         <v>431</v>
       </c>
@@ -9175,7 +9207,7 @@
       </c>
       <c r="N2" s="8"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="63" t="s">
         <v>451</v>
       </c>
@@ -9211,7 +9243,7 @@
       </c>
       <c r="N3" s="12"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="21" t="s">
         <v>439</v>
       </c>
@@ -9247,7 +9279,7 @@
       </c>
       <c r="N4" s="12"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="21" t="s">
         <v>443</v>
       </c>
@@ -9283,7 +9315,7 @@
       </c>
       <c r="N5" s="12"/>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="59" t="s">
         <v>431</v>
       </c>
@@ -9319,7 +9351,7 @@
       </c>
       <c r="N6" s="12"/>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="21" t="s">
         <v>447</v>
       </c>
@@ -9355,7 +9387,7 @@
       </c>
       <c r="N7" s="12"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="59" t="s">
         <v>431</v>
       </c>
@@ -9391,7 +9423,7 @@
       </c>
       <c r="N8" s="12"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="21" t="s">
         <v>435</v>
       </c>
@@ -9427,7 +9459,7 @@
       </c>
       <c r="N9" s="12"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="21" t="s">
         <v>439</v>
       </c>
@@ -9463,7 +9495,7 @@
       </c>
       <c r="N10" s="12"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="21" t="s">
         <v>443</v>
       </c>
@@ -9499,7 +9531,7 @@
       </c>
       <c r="N11" s="12"/>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="59" t="s">
         <v>431</v>
       </c>
@@ -9535,7 +9567,7 @@
       </c>
       <c r="N12" s="12"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="21" t="s">
         <v>447</v>
       </c>
@@ -9571,7 +9603,7 @@
       </c>
       <c r="N13" s="12"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="59" t="s">
         <v>431</v>
       </c>
@@ -9607,7 +9639,7 @@
       </c>
       <c r="N14" s="12"/>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="21" t="s">
         <v>443</v>
       </c>
@@ -9643,7 +9675,7 @@
       </c>
       <c r="N15" s="12"/>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="59" t="s">
         <v>431</v>
       </c>
@@ -9679,7 +9711,7 @@
       </c>
       <c r="N16" s="12"/>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="61" t="s">
         <v>451</v>
       </c>
@@ -9715,7 +9747,7 @@
       </c>
       <c r="N17" s="12"/>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="61" t="s">
         <v>451</v>
       </c>
@@ -9751,7 +9783,7 @@
       </c>
       <c r="N18" s="12"/>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="21" t="s">
         <v>447</v>
       </c>
@@ -9787,7 +9819,7 @@
       </c>
       <c r="N19" s="12"/>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="21" t="s">
         <v>439</v>
       </c>
@@ -9823,7 +9855,7 @@
       </c>
       <c r="N20" s="12"/>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="21" t="s">
         <v>443</v>
       </c>
@@ -9859,7 +9891,7 @@
       </c>
       <c r="N21" s="12"/>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="59" t="s">
         <v>431</v>
       </c>
@@ -9895,7 +9927,7 @@
       </c>
       <c r="N22" s="12"/>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="21" t="s">
         <v>455</v>
       </c>
@@ -9931,7 +9963,7 @@
       </c>
       <c r="N23" s="12"/>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="61" t="s">
         <v>459</v>
       </c>
@@ -9967,7 +9999,7 @@
       </c>
       <c r="N24" s="12"/>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="21" t="s">
         <v>455</v>
       </c>
@@ -10003,7 +10035,7 @@
       </c>
       <c r="N25" s="12"/>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="59" t="s">
         <v>463</v>
       </c>
@@ -10039,7 +10071,7 @@
       </c>
       <c r="N26" s="12"/>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="61" t="s">
         <v>459</v>
       </c>
@@ -10075,7 +10107,7 @@
       </c>
       <c r="N27" s="12"/>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="61" t="s">
         <v>459</v>
       </c>
@@ -10111,7 +10143,7 @@
       </c>
       <c r="N28" s="12"/>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="21" t="s">
         <v>471</v>
       </c>
@@ -10147,7 +10179,7 @@
       </c>
       <c r="N29" s="12"/>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" s="59" t="s">
         <v>463</v>
       </c>
@@ -10183,7 +10215,7 @@
       </c>
       <c r="N30" s="12"/>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" s="21" t="s">
         <v>467</v>
       </c>
@@ -10219,7 +10251,7 @@
       </c>
       <c r="N31" s="12"/>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" s="21" t="s">
         <v>455</v>
       </c>
@@ -10255,7 +10287,7 @@
       </c>
       <c r="N32" s="12"/>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" s="59" t="s">
         <v>463</v>
       </c>
@@ -10291,7 +10323,7 @@
       </c>
       <c r="N33" s="12"/>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" s="61" t="s">
         <v>459</v>
       </c>
@@ -10327,7 +10359,7 @@
       </c>
       <c r="N34" s="12"/>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" s="61" t="s">
         <v>459</v>
       </c>
@@ -10363,7 +10395,7 @@
       </c>
       <c r="N35" s="12"/>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" s="21" t="s">
         <v>471</v>
       </c>
@@ -10399,7 +10431,7 @@
       </c>
       <c r="N36" s="12"/>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" s="59" t="s">
         <v>463</v>
       </c>
@@ -10435,7 +10467,7 @@
       </c>
       <c r="N37" s="12"/>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" s="21" t="s">
         <v>467</v>
       </c>
@@ -10471,7 +10503,7 @@
       </c>
       <c r="N38" s="12"/>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" s="21" t="s">
         <v>455</v>
       </c>
@@ -10507,7 +10539,7 @@
       </c>
       <c r="N39" s="12"/>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" s="59" t="s">
         <v>463</v>
       </c>
@@ -10543,7 +10575,7 @@
       </c>
       <c r="N40" s="12"/>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41" s="61" t="s">
         <v>459</v>
       </c>
@@ -10579,7 +10611,7 @@
       </c>
       <c r="N41" s="12"/>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42" s="61" t="s">
         <v>459</v>
       </c>
@@ -10615,7 +10647,7 @@
       </c>
       <c r="N42" s="12"/>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43" s="21" t="s">
         <v>471</v>
       </c>
@@ -10651,7 +10683,7 @@
       </c>
       <c r="N43" s="12"/>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A44" s="59" t="s">
         <v>475</v>
       </c>
@@ -10687,7 +10719,7 @@
       </c>
       <c r="N44" s="12"/>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45" s="21" t="s">
         <v>479</v>
       </c>
@@ -10723,7 +10755,7 @@
       </c>
       <c r="N45" s="12"/>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A46" s="21" t="s">
         <v>483</v>
       </c>
@@ -10759,7 +10791,7 @@
       </c>
       <c r="N46" s="12"/>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47" s="59" t="s">
         <v>475</v>
       </c>
@@ -10795,7 +10827,7 @@
       </c>
       <c r="N47" s="12"/>
     </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A48" s="61" t="s">
         <v>487</v>
       </c>
@@ -10831,7 +10863,7 @@
       </c>
       <c r="N48" s="12"/>
     </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A49" s="21" t="s">
         <v>491</v>
       </c>
@@ -10867,7 +10899,7 @@
       </c>
       <c r="N49" s="12"/>
     </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A50" s="59" t="s">
         <v>495</v>
       </c>
@@ -10903,7 +10935,7 @@
       </c>
       <c r="N50" s="12"/>
     </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A51" s="21" t="s">
         <v>499</v>
       </c>
@@ -10939,7 +10971,7 @@
       </c>
       <c r="N51" s="12"/>
     </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A52" s="21" t="s">
         <v>503</v>
       </c>
@@ -10975,7 +11007,7 @@
       </c>
       <c r="N52" s="12"/>
     </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A53" s="21" t="s">
         <v>507</v>
       </c>
@@ -11011,7 +11043,7 @@
       </c>
       <c r="N53" s="12"/>
     </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A54" s="59" t="s">
         <v>495</v>
       </c>
@@ -11047,7 +11079,7 @@
       </c>
       <c r="N54" s="12"/>
     </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A55" s="61" t="s">
         <v>511</v>
       </c>
@@ -11083,7 +11115,7 @@
       </c>
       <c r="N55" s="12"/>
     </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A56" s="21" t="s">
         <v>515</v>
       </c>
@@ -11119,7 +11151,7 @@
       </c>
       <c r="N56" s="12"/>
     </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A57" s="59" t="s">
         <v>519</v>
       </c>
@@ -11155,7 +11187,7 @@
       </c>
       <c r="N57" s="12"/>
     </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A58" s="21" t="s">
         <v>523</v>
       </c>
@@ -11191,7 +11223,7 @@
       </c>
       <c r="N58" s="12"/>
     </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A59" s="21" t="s">
         <v>527</v>
       </c>
@@ -11227,7 +11259,7 @@
       </c>
       <c r="N59" s="12"/>
     </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A60" s="59" t="s">
         <v>519</v>
       </c>
@@ -11263,7 +11295,7 @@
       </c>
       <c r="N60" s="12"/>
     </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A61" s="61" t="s">
         <v>531</v>
       </c>
@@ -11299,7 +11331,7 @@
       </c>
       <c r="N61" s="12"/>
     </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A62" s="61" t="s">
         <v>531</v>
       </c>
@@ -11335,7 +11367,7 @@
       </c>
       <c r="N62" s="12"/>
     </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A63" s="21" t="s">
         <v>535</v>
       </c>
@@ -11371,7 +11403,7 @@
       </c>
       <c r="N63" s="12"/>
     </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A64" s="21" t="s">
         <v>483</v>
       </c>
@@ -11407,7 +11439,7 @@
       </c>
       <c r="N64" s="12"/>
     </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A65" s="21" t="s">
         <v>479</v>
       </c>
@@ -11443,7 +11475,7 @@
       </c>
       <c r="N65" s="12"/>
     </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A66" s="21" t="s">
         <v>483</v>
       </c>
@@ -11479,7 +11511,7 @@
       </c>
       <c r="N66" s="12"/>
     </row>
-    <row r="67" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A67" s="60" t="s">
         <v>475</v>
       </c>
@@ -11531,21 +11563,21 @@
       <selection pane="bottomLeft" activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.3046875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.07421875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.69140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.07421875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.53515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.07421875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="34.07421875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.69140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.53515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="34.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="13" t="s">
         <v>132</v>
       </c>
@@ -11580,7 +11612,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="30" t="s">
         <v>549</v>
       </c>
@@ -11611,7 +11643,7 @@
       </c>
       <c r="K2" s="47"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="21" t="s">
         <v>560</v>
       </c>
@@ -11642,7 +11674,7 @@
       </c>
       <c r="K3" s="49"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="21" t="s">
         <v>573</v>
       </c>
@@ -11673,7 +11705,7 @@
       </c>
       <c r="K4" s="49"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="21" t="s">
         <v>586</v>
       </c>
@@ -11704,7 +11736,7 @@
       </c>
       <c r="K5" s="49"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="21" t="s">
         <v>593</v>
       </c>
@@ -11735,7 +11767,7 @@
       </c>
       <c r="K6" s="49"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="21" t="s">
         <v>598</v>
       </c>
@@ -11766,7 +11798,7 @@
       </c>
       <c r="K7" s="49"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="21" t="s">
         <v>609</v>
       </c>
@@ -11797,7 +11829,7 @@
       </c>
       <c r="K8" s="49"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="21" t="s">
         <v>624</v>
       </c>
@@ -11828,7 +11860,7 @@
       </c>
       <c r="K9" s="49"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="21" t="s">
         <v>639</v>
       </c>
@@ -11859,7 +11891,7 @@
       </c>
       <c r="K10" s="49"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="21" t="s">
         <v>652</v>
       </c>
@@ -11890,7 +11922,7 @@
       </c>
       <c r="K11" s="49"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="21" t="s">
         <v>667</v>
       </c>
@@ -11921,7 +11953,7 @@
       </c>
       <c r="K12" s="49"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="21" t="s">
         <v>682</v>
       </c>
@@ -11952,7 +11984,7 @@
       </c>
       <c r="K13" s="49"/>
     </row>
-    <row r="14" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="38" t="s">
         <v>685</v>
       </c>

</xml_diff>